<commit_message>
chore: Torna pipeline idempotente e adiciona .gitignore
Melhora a robustez e as boas práticas do projeto com duas alterações principais:

1.  **Idempotência do Pipeline:** O script de ETL () agora remove o diretório do data lake antes de cada execução. Isso garante que o pipeline possa ser executado várias vezes sem causar erros ou duplicação de dados.

2.  **Criação do .gitignore:** Adicionado um arquivo  para projetos Python, que impede o versionamento de arquivos de cache, ambientes virtuais e os diretórios de saída ( e ).
</commit_message>
<xml_diff>
--- a/data/launches_for_analysis.xlsx
+++ b/data/launches_for_analysis.xlsx
@@ -1856,10 +1856,10 @@
         <v>50000000</v>
       </c>
       <c r="J33" t="n">
-        <v>3.2559</v>
+        <v>3.2537</v>
       </c>
       <c r="K33" t="n">
-        <v>162795000</v>
+        <v>162685000</v>
       </c>
     </row>
     <row r="34">

</xml_diff>